<commit_message>
Fix Excel sheet and Sales Estimate graph
</commit_message>
<xml_diff>
--- a/PS VR2 Sales Estimate.xlsx
+++ b/PS VR2 Sales Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aledb\Dropbox (Personal)\Alex\Programming in Python\estimate-PSVR2-sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDC0BF-1C7A-4076-BC46-D49BF97D0DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C76922E-5EC8-4E74-83DA-B22BA80889BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20010" yWindow="105" windowWidth="18165" windowHeight="15375" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
+    <workbookView xWindow="6645" yWindow="15" windowWidth="24405" windowHeight="15375" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated PS VR2 Sales" sheetId="5" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,12 +175,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -338,10 +332,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$30</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="29"/>
+                  <c:ptCount val="30"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -429,15 +423,18 @@
                   <c:pt idx="28">
                     <c:v>113528.11503984376</c:v>
                   </c:pt>
+                  <c:pt idx="29">
+                    <c:v>120869.2976421225</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$30</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="29"/>
+                  <c:ptCount val="30"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -525,6 +522,9 @@
                   <c:pt idx="28">
                     <c:v>113528.11503984376</c:v>
                   </c:pt>
+                  <c:pt idx="29">
+                    <c:v>120869.2976421225</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
@@ -544,10 +544,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$30</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44979.791666666664</c:v>
                 </c:pt>
@@ -634,16 +634,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45201</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$30</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>437221.74996356922</c:v>
                 </c:pt>
@@ -730,6 +733,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>838458.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>853664.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -756,6 +762,7 @@
         <c:axId val="1022667008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="45218"/>
           <c:min val="44978"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -9678,7 +9685,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9720,15 +9727,15 @@
         <v>436152.78661883302</v>
       </c>
       <c r="D2" s="17">
-        <f>AVERAGE(B2:C2)</f>
+        <f t="shared" ref="D2:D16" si="0">AVERAGE(B2:C2)</f>
         <v>437221.74996356922</v>
       </c>
       <c r="E2" s="15">
-        <f>STDEV(B2:C2)*2</f>
+        <f t="shared" ref="E2:E16" si="1">STDEV(B2:C2)*2</f>
         <v>3023.484919611361</v>
       </c>
       <c r="F2" s="15">
-        <f>STDEV(B2:C2)</f>
+        <f t="shared" ref="F2:F16" si="2">STDEV(B2:C2)</f>
         <v>1511.7424598056805</v>
       </c>
     </row>
@@ -9743,15 +9750,15 @@
         <v>504280.48190166097</v>
       </c>
       <c r="D3" s="17">
-        <f>AVERAGE(B3:C3)</f>
+        <f t="shared" si="0"/>
         <v>502628.310008378</v>
       </c>
       <c r="E3" s="15">
-        <f>STDEV(B3:C3)*2</f>
+        <f t="shared" si="1"/>
         <v>4673.0477977048968</v>
       </c>
       <c r="F3" s="15">
-        <f>STDEV(B3:C3)</f>
+        <f t="shared" si="2"/>
         <v>2336.5238988524484</v>
       </c>
     </row>
@@ -9766,15 +9773,15 @@
         <v>533696.10593416519</v>
       </c>
       <c r="D4" s="17">
-        <f>AVERAGE(B4:C4)</f>
+        <f t="shared" si="0"/>
         <v>533344.70188799629</v>
       </c>
       <c r="E4" s="15">
-        <f>STDEV(B4:C4)*2</f>
+        <f t="shared" si="1"/>
         <v>993.92073592967949</v>
       </c>
       <c r="F4" s="15">
-        <f>STDEV(B4:C4)</f>
+        <f t="shared" si="2"/>
         <v>496.96036796483975</v>
       </c>
     </row>
@@ -9789,15 +9796,15 @@
         <v>549930.20032946218</v>
       </c>
       <c r="D5" s="17">
-        <f>AVERAGE(B5:C5)</f>
+        <f t="shared" si="0"/>
         <v>552711.02142206416</v>
       </c>
       <c r="E5" s="15">
-        <f>STDEV(B5:C5)*2</f>
+        <f t="shared" si="1"/>
         <v>7865.3498073819474</v>
       </c>
       <c r="F5" s="15">
-        <f>STDEV(B5:C5)</f>
+        <f t="shared" si="2"/>
         <v>3932.6749036909737</v>
       </c>
     </row>
@@ -9812,15 +9819,15 @@
         <v>570604.38891834486</v>
       </c>
       <c r="D6" s="17">
-        <f>AVERAGE(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>571084.21920117619</v>
       </c>
       <c r="E6" s="15">
-        <f>STDEV(B6:C6)*2</f>
+        <f t="shared" si="1"/>
         <v>1357.1649872347748</v>
       </c>
       <c r="F6" s="15">
-        <f>STDEV(B6:C6)</f>
+        <f t="shared" si="2"/>
         <v>678.5824936173874</v>
       </c>
     </row>
@@ -9835,15 +9842,15 @@
         <v>582537.14206360595</v>
       </c>
       <c r="D7" s="17">
-        <f>AVERAGE(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>583610.55039985222</v>
       </c>
       <c r="E7" s="15">
-        <f>STDEV(B7:C7)*2</f>
+        <f t="shared" si="1"/>
         <v>3036.0572541674637</v>
       </c>
       <c r="F7" s="15">
-        <f>STDEV(B7:C7)</f>
+        <f t="shared" si="2"/>
         <v>1518.0286270837319</v>
       </c>
     </row>
@@ -9858,15 +9865,15 @@
         <v>592527.35399917339</v>
       </c>
       <c r="D8" s="17">
-        <f>AVERAGE(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>594281.1942206258</v>
       </c>
       <c r="E8" s="15">
-        <f>STDEV(B8:C8)*2</f>
+        <f t="shared" si="1"/>
         <v>4960.6092548270271</v>
       </c>
       <c r="F8" s="15">
-        <f>STDEV(B8:C8)</f>
+        <f t="shared" si="2"/>
         <v>2480.3046274135136</v>
       </c>
     </row>
@@ -9881,15 +9888,15 @@
         <v>595996.17758791195</v>
       </c>
       <c r="D9" s="17">
-        <f>AVERAGE(B9:C9)</f>
+        <f t="shared" si="0"/>
         <v>600857.62877970957</v>
       </c>
       <c r="E9" s="15">
-        <f>STDEV(B9:C9)*2</f>
+        <f t="shared" si="1"/>
         <v>13750.26041651008</v>
       </c>
       <c r="F9" s="15">
-        <f>STDEV(B9:C9)</f>
+        <f t="shared" si="2"/>
         <v>6875.1302082550401</v>
       </c>
     </row>
@@ -9904,15 +9911,15 @@
         <v>613062.78964450595</v>
       </c>
       <c r="D10" s="17">
-        <f>AVERAGE(B10:C10)</f>
+        <f t="shared" si="0"/>
         <v>614315.67281048885</v>
       </c>
       <c r="E10" s="15">
-        <f>STDEV(B10:C10)*2</f>
+        <f t="shared" si="1"/>
         <v>3543.688730804085</v>
       </c>
       <c r="F10" s="15">
-        <f>STDEV(B10:C10)</f>
+        <f t="shared" si="2"/>
         <v>1771.8443654020425</v>
       </c>
     </row>
@@ -9927,15 +9934,15 @@
         <v>621526.71920102881</v>
       </c>
       <c r="D11" s="17">
-        <f>AVERAGE(B11:C11)</f>
+        <f t="shared" si="0"/>
         <v>622651.58592415205</v>
       </c>
       <c r="E11" s="15">
-        <f>STDEV(B11:C11)*2</f>
+        <f t="shared" si="1"/>
         <v>3181.6035514061327</v>
       </c>
       <c r="F11" s="15">
-        <f>STDEV(B11:C11)</f>
+        <f t="shared" si="2"/>
         <v>1590.8017757030664</v>
       </c>
     </row>
@@ -9950,15 +9957,15 @@
         <v>632349.44879789359</v>
       </c>
       <c r="D12" s="17">
-        <f>AVERAGE(B12:C12)</f>
+        <f t="shared" si="0"/>
         <v>631727.87202675734</v>
       </c>
       <c r="E12" s="15">
-        <f>STDEV(B12:C12)*2</f>
+        <f t="shared" si="1"/>
         <v>1758.0845995941081</v>
       </c>
       <c r="F12" s="15">
-        <f>STDEV(B12:C12)</f>
+        <f t="shared" si="2"/>
         <v>879.04229979705406</v>
       </c>
     </row>
@@ -9973,15 +9980,15 @@
         <v>643310.93133830791</v>
       </c>
       <c r="D13" s="17">
-        <f>AVERAGE(B13:C13)</f>
+        <f t="shared" si="0"/>
         <v>640669.92786201672</v>
       </c>
       <c r="E13" s="15">
-        <f>STDEV(B13:C13)*2</f>
+        <f t="shared" si="1"/>
         <v>7469.8858688910013</v>
       </c>
       <c r="F13" s="15">
-        <f>STDEV(B13:C13)</f>
+        <f t="shared" si="2"/>
         <v>3734.9429344455007</v>
       </c>
     </row>
@@ -9996,15 +10003,15 @@
         <v>661626.3198868481</v>
       </c>
       <c r="D14" s="17">
-        <f>AVERAGE(B14:C14)</f>
+        <f t="shared" si="0"/>
         <v>653638.8857842026</v>
       </c>
       <c r="E14" s="15">
-        <f>STDEV(B14:C14)*2</f>
+        <f t="shared" si="1"/>
         <v>22591.875273045258</v>
       </c>
       <c r="F14" s="15">
-        <f>STDEV(B14:C14)</f>
+        <f t="shared" si="2"/>
         <v>11295.937636522629</v>
       </c>
     </row>
@@ -10019,15 +10026,15 @@
         <v>674114.08480630745</v>
       </c>
       <c r="D15" s="17">
-        <f>AVERAGE(B15:C15)</f>
+        <f t="shared" si="0"/>
         <v>663821.28610379866</v>
       </c>
       <c r="E15" s="15">
-        <f>STDEV(B15:C15)*2</f>
+        <f t="shared" si="1"/>
         <v>29112.431039728261</v>
       </c>
       <c r="F15" s="15">
-        <f>STDEV(B15:C15)</f>
+        <f t="shared" si="2"/>
         <v>14556.21551986413</v>
       </c>
     </row>
@@ -10042,15 +10049,15 @@
         <v>688960.64976610907</v>
       </c>
       <c r="D16" s="17">
-        <f>AVERAGE(B16:C16)</f>
+        <f t="shared" si="0"/>
         <v>675246.71354954084</v>
       </c>
       <c r="E16" s="15">
-        <f>STDEV(B16:C16)*2</f>
+        <f t="shared" si="1"/>
         <v>38788.869181980546</v>
       </c>
       <c r="F16" s="15">
-        <f>STDEV(B16:C16)</f>
+        <f t="shared" si="2"/>
         <v>19394.434590990273</v>
       </c>
     </row>
@@ -10137,15 +10144,15 @@
         <v>787058</v>
       </c>
       <c r="D21" s="17">
-        <f>AVERAGE(B21:C21)</f>
+        <f t="shared" ref="D21:D31" si="3">AVERAGE(B21:C21)</f>
         <v>744719.5</v>
       </c>
       <c r="E21" s="15">
-        <f>STDEV(B21:C21)*2</f>
+        <f t="shared" ref="E21:E31" si="4">STDEV(B21:C21)*2</f>
         <v>119751.36182106657</v>
       </c>
       <c r="F21" s="15">
-        <f>STDEV(B21:C21)</f>
+        <f t="shared" ref="F21:F31" si="5">STDEV(B21:C21)</f>
         <v>59875.680910533287</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -10163,15 +10170,15 @@
         <v>800101</v>
       </c>
       <c r="D22" s="17">
-        <f>AVERAGE(B22:C22)</f>
+        <f t="shared" si="3"/>
         <v>754199.5</v>
       </c>
       <c r="E22" s="15">
-        <f>STDEV(B22:C22)*2</f>
+        <f t="shared" si="4"/>
         <v>129829.04766653724</v>
       </c>
       <c r="F22" s="15">
-        <f>STDEV(B22:C22)</f>
+        <f t="shared" si="5"/>
         <v>64914.52383326862</v>
       </c>
       <c r="H22" t="s">
@@ -10189,15 +10196,15 @@
         <v>817029</v>
       </c>
       <c r="D23" s="17">
-        <f>AVERAGE(B23:C23)</f>
+        <f t="shared" si="3"/>
         <v>765921.5</v>
       </c>
       <c r="E23" s="15">
-        <f>STDEV(B23:C23)*2</f>
+        <f t="shared" si="4"/>
         <v>144553.83927796592</v>
       </c>
       <c r="F23" s="15">
-        <f>STDEV(B23:C23)</f>
+        <f t="shared" si="5"/>
         <v>72276.919638982959</v>
       </c>
       <c r="H23" cm="1">
@@ -10219,15 +10226,15 @@
         <v>829101</v>
       </c>
       <c r="D24" s="17">
-        <f>AVERAGE(B24:C24)</f>
+        <f t="shared" si="3"/>
         <v>775030.5</v>
       </c>
       <c r="E24" s="15">
-        <f>STDEV(B24:C24)*2</f>
+        <f t="shared" si="4"/>
         <v>152934.46884858888</v>
       </c>
       <c r="F24" s="15">
-        <f>STDEV(B24:C24)</f>
+        <f t="shared" si="5"/>
         <v>76467.234424294438</v>
       </c>
       <c r="H24" t="s">
@@ -10245,15 +10252,15 @@
         <v>838536</v>
       </c>
       <c r="D25" s="17">
-        <f>AVERAGE(B25:C25)</f>
+        <f t="shared" si="3"/>
         <v>782216.5</v>
       </c>
       <c r="E25" s="15">
-        <f>STDEV(B25:C25)*2</f>
+        <f t="shared" si="4"/>
         <v>159295.60145214305</v>
       </c>
       <c r="F25" s="15">
-        <f>STDEV(B25:C25)</f>
+        <f t="shared" si="5"/>
         <v>79647.800726071524</v>
       </c>
       <c r="H25" s="8">
@@ -10272,15 +10279,15 @@
         <v>875583</v>
       </c>
       <c r="D26" s="17">
-        <f>AVERAGE(B26:C26)</f>
+        <f t="shared" si="3"/>
         <v>808852.5</v>
       </c>
       <c r="E26" s="15">
-        <f>STDEV(B26:C26)*2</f>
+        <f t="shared" si="4"/>
         <v>188742.35624787564</v>
       </c>
       <c r="F26" s="15">
-        <f>STDEV(B26:C26)</f>
+        <f t="shared" si="5"/>
         <v>94371.178123937818</v>
       </c>
     </row>
@@ -10295,15 +10302,15 @@
         <v>882659</v>
       </c>
       <c r="D27" s="17">
-        <f>AVERAGE(B27:C27)</f>
+        <f t="shared" si="3"/>
         <v>813892.5</v>
       </c>
       <c r="E27" s="15">
-        <f>STDEV(B27:C27)*2</f>
+        <f t="shared" si="4"/>
         <v>194501.03387385889</v>
       </c>
       <c r="F27" s="15">
-        <f>STDEV(B27:C27)</f>
+        <f t="shared" si="5"/>
         <v>97250.516936929445</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -10321,15 +10328,15 @@
         <v>892372</v>
       </c>
       <c r="D28" s="17">
-        <f>AVERAGE(B28:C28)</f>
+        <f t="shared" si="3"/>
         <v>820206</v>
       </c>
       <c r="E28" s="15">
-        <f>STDEV(B28:C28)*2</f>
+        <f t="shared" si="4"/>
         <v>204116.27188443355</v>
       </c>
       <c r="F28" s="15">
-        <f>STDEV(B28:C28)</f>
+        <f t="shared" si="5"/>
         <v>102058.13594221677</v>
       </c>
       <c r="H28" t="s">
@@ -10347,15 +10354,15 @@
         <v>900697</v>
       </c>
       <c r="D29" s="17">
-        <f>AVERAGE(B29:C29)</f>
+        <f t="shared" si="3"/>
         <v>825253</v>
       </c>
       <c r="E29" s="15">
-        <f>STDEV(B29:C29)*2</f>
+        <f t="shared" si="4"/>
         <v>213387.85599935157</v>
       </c>
       <c r="F29" s="15">
-        <f>STDEV(B29:C29)</f>
+        <f t="shared" si="5"/>
         <v>106693.92799967578</v>
       </c>
       <c r="H29">
@@ -10378,15 +10385,15 @@
         <v>918735</v>
       </c>
       <c r="D30" s="17">
-        <f>AVERAGE(B30:C30)</f>
+        <f t="shared" si="3"/>
         <v>838458.5</v>
       </c>
       <c r="E30" s="15">
-        <f>STDEV(B30:C30)*2</f>
+        <f t="shared" si="4"/>
         <v>227056.23007968752</v>
       </c>
       <c r="F30" s="15">
-        <f>STDEV(B30:C30)</f>
+        <f t="shared" si="5"/>
         <v>113528.11503984376</v>
       </c>
       <c r="H30" t="s">
@@ -10404,15 +10411,15 @@
         <v>939132</v>
       </c>
       <c r="D31" s="17">
-        <f>AVERAGE(B31:C31)</f>
+        <f t="shared" si="3"/>
         <v>853664.5</v>
       </c>
       <c r="E31" s="15">
-        <f>STDEV(B31:C31)*2</f>
+        <f t="shared" si="4"/>
         <v>241738.59528424501</v>
       </c>
       <c r="F31" s="15">
-        <f>STDEV(B31:C31)</f>
+        <f t="shared" si="5"/>
         <v>120869.2976421225</v>
       </c>
       <c r="H31" s="8">

</xml_diff>

<commit_message>
Update header description and Excel workbook formatting
</commit_message>
<xml_diff>
--- a/PS VR2 Sales Estimate.xlsx
+++ b/PS VR2 Sales Estimate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aledb\Dropbox (Personal)\Alex\Programming in Python\estimate-PSVR2-sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C76922E-5EC8-4E74-83DA-B22BA80889BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDA9E18-F87E-4EC8-AED5-140A5B80CA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="15" windowWidth="24405" windowHeight="15375" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
+    <workbookView xWindow="12285" yWindow="840" windowWidth="24945" windowHeight="14280" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated PS VR2 Sales" sheetId="5" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Week</t>
   </si>
@@ -156,7 +156,10 @@
     <t>Est Sales Combined</t>
   </si>
   <si>
-    <t>Retrospective reality check to determine if subreddit membership correlates to sales over a period of years.</t>
+    <t>Retrospective reality check to determine if subreddit membership correlates linearly to sales over a period of years.</t>
+  </si>
+  <si>
+    <t>Prediction from first 6 months exhibits 5.2% error 1 year later, and ~25.9% 2 years later, suggesting reasonable linearity.</t>
   </si>
 </sst>
 </file>
@@ -3429,7 +3432,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$B$3:$B$8</c:f>
+              <c:f>'PS5 reality check'!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3456,7 +3459,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$E$3:$E$8</c:f>
+              <c:f>'PS5 reality check'!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3515,7 +3518,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$B$9:$B$12</c:f>
+              <c:f>'PS5 reality check'!$B$10:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3536,7 +3539,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$F$9:$F$12</c:f>
+              <c:f>'PS5 reality check'!$F$10:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3949,7 +3952,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$D$3:$D$8</c:f>
+              <c:f>'PS5 reality check'!$D$4:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3976,7 +3979,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$E$3:$E$12</c:f>
+              <c:f>'PS5 reality check'!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4164,7 +4167,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$D$9:$D$12</c:f>
+              <c:f>'PS5 reality check'!$D$10:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4185,7 +4188,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PS5 reality check'!$F$9:$F$12</c:f>
+              <c:f>'PS5 reality check'!$F$10:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9276,13 +9279,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9314,13 +9317,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9685,20 +9688,20 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="18" customWidth="1"/>
     <col min="5" max="6" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="14" t="s">
         <v>16</v>
@@ -9716,7 +9719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>44979.791666666664</v>
       </c>
@@ -9739,7 +9742,7 @@
         <v>1511.7424598056805</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>44986.791666666664</v>
       </c>
@@ -9762,7 +9765,7 @@
         <v>2336.5238988524484</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>44993.791666666664</v>
       </c>
@@ -9785,7 +9788,7 @@
         <v>496.96036796483975</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>45000.833333333336</v>
       </c>
@@ -9808,7 +9811,7 @@
         <v>3932.6749036909737</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>45007.833333333336</v>
       </c>
@@ -9831,7 +9834,7 @@
         <v>678.5824936173874</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>45014.833333333336</v>
       </c>
@@ -9854,7 +9857,7 @@
         <v>1518.0286270837319</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>45021.833333333336</v>
       </c>
@@ -9877,7 +9880,7 @@
         <v>2480.3046274135136</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>45028.833333333336</v>
       </c>
@@ -9900,7 +9903,7 @@
         <v>6875.1302082550401</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>45035.833333333336</v>
       </c>
@@ -9923,7 +9926,7 @@
         <v>1771.8443654020425</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>45042.833333333336</v>
       </c>
@@ -9946,7 +9949,7 @@
         <v>1590.8017757030664</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>45049.833333333336</v>
       </c>
@@ -9969,7 +9972,7 @@
         <v>879.04229979705406</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>45056.833333333336</v>
       </c>
@@ -9992,7 +9995,7 @@
         <v>3734.9429344455007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>45063.833333333336</v>
       </c>
@@ -10015,7 +10018,7 @@
         <v>11295.937636522629</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>45070.833333333336</v>
       </c>
@@ -10038,7 +10041,7 @@
         <v>14556.21551986413</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>45077.833333333336</v>
       </c>
@@ -10061,7 +10064,7 @@
         <v>19394.434590990273</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>45085</v>
       </c>
@@ -10078,7 +10081,7 @@
         <v>24500</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>45093</v>
       </c>
@@ -10095,7 +10098,7 @@
         <v>35500</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>45100</v>
       </c>
@@ -10112,7 +10115,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>45107</v>
       </c>
@@ -10133,7 +10136,7 @@
         <v>48500</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>45117</v>
       </c>
@@ -10159,7 +10162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>45124</v>
       </c>
@@ -10185,7 +10188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>45131</v>
       </c>
@@ -10215,7 +10218,7 @@
         <v>-44885646.020927444</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>45140</v>
       </c>
@@ -10241,7 +10244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>45146</v>
       </c>
@@ -10268,7 +10271,7 @@
         <v>45259.19742346977</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>45166</v>
       </c>
@@ -10291,7 +10294,7 @@
         <v>94371.178123937818</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>45170</v>
       </c>
@@ -10317,7 +10320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>45176</v>
       </c>
@@ -10343,7 +10346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>45183</v>
       </c>
@@ -10374,7 +10377,7 @@
         <v>-44885646.020927444</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>45201</v>
       </c>
@@ -10400,7 +10403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>45217</v>
       </c>
@@ -10442,23 +10445,23 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="8" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="8" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.5546875" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="22" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -10472,7 +10475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -10486,7 +10489,7 @@
         <v>438000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -10501,7 +10504,7 @@
         <v>498000</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -10516,7 +10519,7 @@
         <v>539000</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -10531,7 +10534,7 @@
         <v>556000</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -10546,7 +10549,7 @@
         <v>569000</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -10561,647 +10564,647 @@
         <v>584000</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E11" s="2"/>
     </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K28" s="2"/>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C37" s="6"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="6"/>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="6"/>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="6"/>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="6"/>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="6"/>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="6"/>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="6"/>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="6"/>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="6"/>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" s="6"/>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" s="6"/>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" s="6"/>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" s="6"/>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" s="6"/>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" s="6"/>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" s="6"/>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C97" s="6"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C99" s="6"/>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C101" s="6"/>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C102" s="6"/>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C103" s="6"/>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C104" s="6"/>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C105" s="6"/>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C106" s="6"/>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C107" s="6"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C108" s="6"/>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C109" s="6"/>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C110" s="6"/>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C112" s="6"/>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C116" s="6"/>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C117" s="6"/>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C119" s="6"/>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C121" s="6"/>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C122" s="6"/>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C123" s="6"/>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C124" s="6"/>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C125" s="6"/>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C126" s="6"/>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C127" s="6"/>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C128" s="6"/>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C129" s="6"/>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C130" s="6"/>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C131" s="6"/>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C132" s="6"/>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C133" s="6"/>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C134" s="6"/>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C135" s="6"/>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C137" s="6"/>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C152" s="6"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C164" s="6"/>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C165" s="6"/>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C166" s="6"/>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C167" s="6"/>
       <c r="D167" s="7"/>
       <c r="Y167" s="6"/>
       <c r="Z167" s="7"/>
     </row>
-    <row r="168" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C168" s="6"/>
       <c r="D168" s="7"/>
       <c r="Y168" s="6"/>
       <c r="Z168" s="7"/>
     </row>
-    <row r="169" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C169" s="6"/>
       <c r="D169" s="7"/>
       <c r="Y169" s="6"/>
       <c r="Z169" s="7"/>
     </row>
-    <row r="170" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C170" s="6"/>
       <c r="D170" s="7"/>
       <c r="Y170" s="6"/>
       <c r="Z170" s="7"/>
     </row>
-    <row r="171" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
       <c r="Y171" s="6"/>
       <c r="Z171" s="7"/>
     </row>
-    <row r="172" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
       <c r="Y172" s="6"/>
       <c r="Z172" s="7"/>
     </row>
-    <row r="173" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
       <c r="Y173" s="6"/>
       <c r="Z173" s="7"/>
     </row>
-    <row r="174" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C174" s="6"/>
       <c r="D174" s="7"/>
       <c r="Y174" s="8"/>
     </row>
-    <row r="175" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C175" s="6"/>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C176" s="6"/>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C177" s="6"/>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C180" s="6"/>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
       <c r="Y182" s="2"/>
     </row>
-    <row r="183" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C183" s="6"/>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C184" s="6"/>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C185" s="6"/>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C186" s="6"/>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
     </row>
@@ -11221,15 +11224,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -11243,7 +11246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -11257,7 +11260,7 @@
         <v>438000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -11272,7 +11275,7 @@
         <v>498000</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -11287,7 +11290,7 @@
         <v>539000</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -11302,7 +11305,7 @@
         <v>556000</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -11317,7 +11320,7 @@
         <v>569000</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -11332,624 +11335,624 @@
         <v>584000</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E11" s="2"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28" s="2"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="6"/>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="6"/>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="6"/>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="6"/>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="6"/>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="6"/>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="6"/>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="6"/>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="6"/>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" s="6"/>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" s="6"/>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" s="6"/>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" s="6"/>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" s="6"/>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" s="6"/>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" s="6"/>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C97" s="6"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C99" s="6"/>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C101" s="6"/>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C102" s="6"/>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C103" s="6"/>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C104" s="6"/>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C105" s="6"/>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C106" s="6"/>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C107" s="6"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C108" s="6"/>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C109" s="6"/>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C110" s="6"/>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C112" s="6"/>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C116" s="6"/>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C117" s="6"/>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C119" s="6"/>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C121" s="6"/>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C122" s="6"/>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C123" s="6"/>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C124" s="6"/>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C125" s="6"/>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C126" s="6"/>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C127" s="6"/>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C128" s="6"/>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C129" s="6"/>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C130" s="6"/>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C131" s="6"/>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C132" s="6"/>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C133" s="6"/>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C134" s="6"/>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C135" s="6"/>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C137" s="6"/>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C152" s="6"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C164" s="6"/>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C165" s="6"/>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C166" s="6"/>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C167" s="6"/>
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C168" s="6"/>
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C169" s="6"/>
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C170" s="6"/>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C174" s="6"/>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C175" s="6"/>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C176" s="6"/>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C177" s="6"/>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C180" s="6"/>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C183" s="6"/>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C184" s="6"/>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C185" s="6"/>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C186" s="6"/>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C188" s="6"/>
       <c r="D188" s="7"/>
     </row>
@@ -11963,232 +11966,237 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5ECA9C6-B268-480D-9831-8BD4DDFDD29F}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>44136</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <v>627167</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
         <v>2750000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>(C4-C3)/7</f>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <f>(C5-C4)/7</f>
         <v>4.2857142857142856</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>44166</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>747323</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>4500000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <f>(C5-C4)/7+B4</f>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f>(C6-C5)/7+B5</f>
         <v>8.7142857142857153</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>44197</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>831669</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>5000000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f t="shared" ref="B6:B9" si="0">(C6-C5)/7+B5</f>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f t="shared" ref="B7:B10" si="0">(C7-C6)/7+B6</f>
         <v>13.142857142857144</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>44228</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>953742</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>5800000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>17.142857142857146</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>44256</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>1033342</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>7000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>21.571428571428577</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>44287</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>1116766</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>7900000</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>47.714285714285722</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>44470</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>1620824</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>12500000</v>
-      </c>
-      <c r="F9" s="2">
-        <f>D9*9.914-3282419</f>
-        <v>12786430.136</v>
-      </c>
-      <c r="G9" s="5">
-        <f>(F9-E9)/E9</f>
-        <v>2.2914410879999996E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f>(C10-C3+7)/7</f>
-        <v>70.285714285714292</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44621</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2052758</v>
-      </c>
-      <c r="E10" s="2">
-        <v>18000000</v>
       </c>
       <c r="F10" s="2">
         <f>D10*9.914-3282419</f>
-        <v>17068623.811999999</v>
+        <v>12786430.136</v>
       </c>
       <c r="G10" s="5">
         <f>(F10-E10)/E10</f>
-        <v>-5.1743121555555611E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.2914410879999996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
-        <f>(C11-C3+7)/7</f>
-        <v>122.42857142857143</v>
+        <f>(C11-C4+7)/7</f>
+        <v>70.285714285714292</v>
       </c>
       <c r="C11" s="1">
-        <v>44986</v>
+        <v>44621</v>
       </c>
       <c r="D11" s="2">
-        <v>2941348</v>
+        <v>2052758</v>
       </c>
       <c r="E11" s="2">
-        <v>32000000</v>
+        <v>18000000</v>
       </c>
       <c r="F11" s="2">
         <f>D11*9.914-3282419</f>
-        <v>25878105.072000001</v>
+        <v>17068623.811999999</v>
       </c>
       <c r="G11" s="5">
         <f>(F11-E11)/E11</f>
-        <v>-0.19130921649999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-5.1743121555555611E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12">
-        <f>(C12-C3+7)/7</f>
-        <v>126.85714285714286</v>
+        <f>(C12-C4+7)/7</f>
+        <v>122.42857142857143</v>
       </c>
       <c r="C12" s="1">
-        <v>45017</v>
+        <v>44986</v>
       </c>
       <c r="D12" s="2">
-        <v>3016851</v>
-      </c>
-      <c r="E12" s="3">
-        <v>35942643</v>
+        <v>2941348</v>
+      </c>
+      <c r="E12" s="2">
+        <v>32000000</v>
       </c>
       <c r="F12" s="2">
         <f>D12*9.914-3282419</f>
-        <v>26626641.813999999</v>
+        <v>25878105.072000001</v>
       </c>
       <c r="G12" s="5">
         <f>(F12-E12)/E12</f>
+        <v>-0.19130921649999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>(C13-C4+7)/7</f>
+        <v>126.85714285714286</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45017</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3016851</v>
+      </c>
+      <c r="E13" s="3">
+        <v>35942643</v>
+      </c>
+      <c r="F13" s="2">
+        <f>D13*9.914-3282419</f>
+        <v>26626641.813999999</v>
+      </c>
+      <c r="G13" s="5">
+        <f>(F13-E13)/E13</f>
         <v>-0.25919076641080624</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" cm="1">
-        <f t="array" ref="C35:D35">LINEST(E3:E8,D3:D8)</f>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" cm="1">
+        <f t="array" ref="C36:D36">LINEST(E4:E9,D4:D9)</f>
         <v>9.9142047621025462</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>-3282419.4191012299</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update sales estimate 10-26-2023
</commit_message>
<xml_diff>
--- a/PS VR2 Sales Estimate.xlsx
+++ b/PS VR2 Sales Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aledb\Dropbox (Personal)\Alex\Programming in Python\estimate-PSVR2-sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDA9E18-F87E-4EC8-AED5-140A5B80CA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572B287-81BB-4A63-82F1-91E766E2D640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12285" yWindow="840" windowWidth="24945" windowHeight="14280" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
+    <workbookView xWindow="165" yWindow="435" windowWidth="21795" windowHeight="14280" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated PS VR2 Sales" sheetId="5" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Week</t>
   </si>
@@ -130,21 +130,6 @@
   </si>
   <si>
     <t>66% CI</t>
-  </si>
-  <si>
-    <t>When will it hit 1M?</t>
-  </si>
-  <si>
-    <t>Projected date:</t>
-  </si>
-  <si>
-    <t>Linear extrapolation from past month:</t>
-  </si>
-  <si>
-    <t>When will it hit 900k?</t>
-  </si>
-  <si>
-    <t>Linear extrapolation from past 2 months:</t>
   </si>
   <si>
     <t>Est Sales from r/PSVR</t>
@@ -230,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -266,6 +251,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,10 +329,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$31</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$32</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="30"/>
+                  <c:ptCount val="31"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -429,15 +423,18 @@
                   <c:pt idx="29">
                     <c:v>120869.2976421225</c:v>
                   </c:pt>
+                  <c:pt idx="30">
+                    <c:v>124616.9635824112</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$31</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$32</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="30"/>
+                  <c:ptCount val="31"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -528,6 +525,9 @@
                   <c:pt idx="29">
                     <c:v>120869.2976421225</c:v>
                   </c:pt>
+                  <c:pt idx="30">
+                    <c:v>124616.9635824112</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
@@ -547,10 +547,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$31</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44979.791666666664</c:v>
                 </c:pt>
@@ -640,16 +640,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45217</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$31</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>437221.74996356922</c:v>
                 </c:pt>
@@ -739,6 +742,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>853664.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>860310.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,7 +771,7 @@
         <c:axId val="1022667008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45218"/>
+          <c:max val="45228"/>
           <c:min val="44978"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -9685,32 +9691,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0C3A37-78ED-4113-9465-0FC068733B9F}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="18" customWidth="1"/>
     <col min="5" max="6" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>9</v>
@@ -9719,7 +9725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>44979.791666666664</v>
       </c>
@@ -9742,7 +9748,7 @@
         <v>1511.7424598056805</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>44986.791666666664</v>
       </c>
@@ -9765,7 +9771,7 @@
         <v>2336.5238988524484</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>44993.791666666664</v>
       </c>
@@ -9788,7 +9794,7 @@
         <v>496.96036796483975</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>45000.833333333336</v>
       </c>
@@ -9811,7 +9817,7 @@
         <v>3932.6749036909737</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>45007.833333333336</v>
       </c>
@@ -9834,7 +9840,7 @@
         <v>678.5824936173874</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>45014.833333333336</v>
       </c>
@@ -9857,7 +9863,7 @@
         <v>1518.0286270837319</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>45021.833333333336</v>
       </c>
@@ -9880,7 +9886,7 @@
         <v>2480.3046274135136</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>45028.833333333336</v>
       </c>
@@ -9903,7 +9909,7 @@
         <v>6875.1302082550401</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>45035.833333333336</v>
       </c>
@@ -9926,7 +9932,7 @@
         <v>1771.8443654020425</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>45042.833333333336</v>
       </c>
@@ -9949,7 +9955,7 @@
         <v>1590.8017757030664</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>45049.833333333336</v>
       </c>
@@ -9972,7 +9978,7 @@
         <v>879.04229979705406</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>45056.833333333336</v>
       </c>
@@ -9995,7 +10001,7 @@
         <v>3734.9429344455007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>45063.833333333336</v>
       </c>
@@ -10018,7 +10024,7 @@
         <v>11295.937636522629</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>45070.833333333336</v>
       </c>
@@ -10041,7 +10047,7 @@
         <v>14556.21551986413</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>45077.833333333336</v>
       </c>
@@ -10064,7 +10070,7 @@
         <v>19394.434590990273</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>45085</v>
       </c>
@@ -10081,7 +10087,7 @@
         <v>24500</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>45093</v>
       </c>
@@ -10098,7 +10104,7 @@
         <v>35500</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>45100</v>
       </c>
@@ -10115,7 +10121,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>45107</v>
       </c>
@@ -10136,7 +10142,7 @@
         <v>48500</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>45117</v>
       </c>
@@ -10147,22 +10153,20 @@
         <v>787058</v>
       </c>
       <c r="D21" s="17">
-        <f t="shared" ref="D21:D31" si="3">AVERAGE(B21:C21)</f>
+        <f t="shared" ref="D21:D32" si="3">AVERAGE(B21:C21)</f>
         <v>744719.5</v>
       </c>
       <c r="E21" s="15">
-        <f t="shared" ref="E21:E31" si="4">STDEV(B21:C21)*2</f>
+        <f t="shared" ref="E21:E32" si="4">STDEV(B21:C21)*2</f>
         <v>119751.36182106657</v>
       </c>
       <c r="F21" s="15">
-        <f t="shared" ref="F21:F31" si="5">STDEV(B21:C21)</f>
+        <f t="shared" ref="F21:F32" si="5">STDEV(B21:C21)</f>
         <v>59875.680910533287</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>45124</v>
       </c>
@@ -10184,11 +10188,8 @@
         <f t="shared" si="5"/>
         <v>64914.52383326862</v>
       </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>45131</v>
       </c>
@@ -10210,15 +10211,8 @@
         <f t="shared" si="5"/>
         <v>72276.919638982959</v>
       </c>
-      <c r="H23" cm="1">
-        <f t="array" ref="H23:I23">LINEST(D24:D31,A24:A31)</f>
-        <v>1011.6318588801284</v>
-      </c>
-      <c r="I23">
-        <v>-44885646.020927444</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>45140</v>
       </c>
@@ -10240,11 +10234,8 @@
         <f t="shared" si="5"/>
         <v>76467.234424294438</v>
       </c>
-      <c r="H24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>45146</v>
       </c>
@@ -10266,12 +10257,9 @@
         <f t="shared" si="5"/>
         <v>79647.800726071524</v>
       </c>
-      <c r="H25" s="8">
-        <f>(900000-I23)/H23</f>
-        <v>45259.19742346977</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>45166</v>
       </c>
@@ -10294,7 +10282,7 @@
         <v>94371.178123937818</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>45170</v>
       </c>
@@ -10316,11 +10304,9 @@
         <f t="shared" si="5"/>
         <v>97250.516936929445</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>45176</v>
       </c>
@@ -10342,11 +10328,8 @@
         <f t="shared" si="5"/>
         <v>102058.13594221677</v>
       </c>
-      <c r="H28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>45183</v>
       </c>
@@ -10368,16 +10351,8 @@
         <f t="shared" si="5"/>
         <v>106693.92799967578</v>
       </c>
-      <c r="H29">
-        <f>H23</f>
-        <v>1011.6318588801284</v>
-      </c>
-      <c r="I29">
-        <f>I23</f>
-        <v>-44885646.020927444</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>45201</v>
       </c>
@@ -10399,11 +10374,8 @@
         <f t="shared" si="5"/>
         <v>113528.11503984376</v>
       </c>
-      <c r="H30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>45217</v>
       </c>
@@ -10425,9 +10397,29 @@
         <f t="shared" si="5"/>
         <v>120869.2976421225</v>
       </c>
-      <c r="H31" s="8">
-        <f>(1000000-I29)/H29</f>
-        <v>45358.04761202621</v>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>45225</v>
+      </c>
+      <c r="B32" s="19">
+        <v>772193</v>
+      </c>
+      <c r="C32" s="19">
+        <v>948428</v>
+      </c>
+      <c r="D32" s="20">
+        <f t="shared" si="3"/>
+        <v>860310.5</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="4"/>
+        <v>249233.92716482241</v>
+      </c>
+      <c r="F32" s="21">
+        <f t="shared" si="5"/>
+        <v>124616.9635824112</v>
       </c>
     </row>
   </sheetData>
@@ -10445,23 +10437,23 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="8" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="8" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="22" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -10475,7 +10467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -10489,7 +10481,7 @@
         <v>438000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -10504,7 +10496,7 @@
         <v>498000</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -10519,7 +10511,7 @@
         <v>539000</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -10534,7 +10526,7 @@
         <v>556000</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -10549,7 +10541,7 @@
         <v>569000</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -10564,647 +10556,647 @@
         <v>584000</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
     </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K28" s="2"/>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" s="6"/>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72" s="6"/>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" s="6"/>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C79" s="6"/>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" s="6"/>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" s="6"/>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85" s="6"/>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C87" s="6"/>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C88" s="6"/>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C89" s="6"/>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90" s="6"/>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C91" s="6"/>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C92" s="6"/>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93" s="6"/>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C95" s="6"/>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C96" s="6"/>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" s="6"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99" s="6"/>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" s="6"/>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102" s="6"/>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103" s="6"/>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104" s="6"/>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C105" s="6"/>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106" s="6"/>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107" s="6"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108" s="6"/>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109" s="6"/>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110" s="6"/>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" s="6"/>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" s="6"/>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" s="6"/>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" s="6"/>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" s="6"/>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" s="6"/>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" s="6"/>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" s="6"/>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" s="6"/>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" s="6"/>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C128" s="6"/>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C129" s="6"/>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C130" s="6"/>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131" s="6"/>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C132" s="6"/>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C133" s="6"/>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C134" s="6"/>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C135" s="6"/>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C137" s="6"/>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C152" s="6"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C164" s="6"/>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C165" s="6"/>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C166" s="6"/>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C167" s="6"/>
       <c r="D167" s="7"/>
       <c r="Y167" s="6"/>
       <c r="Z167" s="7"/>
     </row>
-    <row r="168" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C168" s="6"/>
       <c r="D168" s="7"/>
       <c r="Y168" s="6"/>
       <c r="Z168" s="7"/>
     </row>
-    <row r="169" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C169" s="6"/>
       <c r="D169" s="7"/>
       <c r="Y169" s="6"/>
       <c r="Z169" s="7"/>
     </row>
-    <row r="170" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C170" s="6"/>
       <c r="D170" s="7"/>
       <c r="Y170" s="6"/>
       <c r="Z170" s="7"/>
     </row>
-    <row r="171" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
       <c r="Y171" s="6"/>
       <c r="Z171" s="7"/>
     </row>
-    <row r="172" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
       <c r="Y172" s="6"/>
       <c r="Z172" s="7"/>
     </row>
-    <row r="173" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
       <c r="Y173" s="6"/>
       <c r="Z173" s="7"/>
     </row>
-    <row r="174" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C174" s="6"/>
       <c r="D174" s="7"/>
       <c r="Y174" s="8"/>
     </row>
-    <row r="175" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C175" s="6"/>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="3:26" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C176" s="6"/>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C177" s="6"/>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C180" s="6"/>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
       <c r="Y182" s="2"/>
     </row>
-    <row r="183" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C183" s="6"/>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C184" s="6"/>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C185" s="6"/>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C186" s="6"/>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
     </row>
@@ -11224,15 +11216,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -11246,7 +11238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -11260,7 +11252,7 @@
         <v>438000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -11275,7 +11267,7 @@
         <v>498000</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -11290,7 +11282,7 @@
         <v>539000</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -11305,7 +11297,7 @@
         <v>556000</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -11320,7 +11312,7 @@
         <v>569000</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -11335,624 +11327,624 @@
         <v>584000</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" s="6"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C63" s="6"/>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" s="6"/>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67" s="6"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" s="6"/>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" s="6"/>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72" s="6"/>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" s="6"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="6"/>
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" s="6"/>
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C79" s="6"/>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" s="6"/>
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" s="6"/>
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85" s="6"/>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86" s="6"/>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C87" s="6"/>
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C88" s="6"/>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C89" s="6"/>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90" s="6"/>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C91" s="6"/>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C92" s="6"/>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93" s="6"/>
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C95" s="6"/>
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C96" s="6"/>
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" s="6"/>
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99" s="6"/>
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" s="6"/>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102" s="6"/>
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103" s="6"/>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104" s="6"/>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C105" s="6"/>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106" s="6"/>
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107" s="6"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108" s="6"/>
       <c r="D108" s="7"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109" s="6"/>
       <c r="D109" s="7"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110" s="6"/>
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111" s="6"/>
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" s="6"/>
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" s="6"/>
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" s="6"/>
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" s="6"/>
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" s="6"/>
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" s="6"/>
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" s="6"/>
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" s="6"/>
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" s="6"/>
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" s="6"/>
       <c r="D127" s="7"/>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C128" s="6"/>
       <c r="D128" s="7"/>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C129" s="6"/>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C130" s="6"/>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131" s="6"/>
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C132" s="6"/>
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C133" s="6"/>
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C134" s="6"/>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C135" s="6"/>
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136" s="6"/>
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C137" s="6"/>
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C138" s="6"/>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C139" s="6"/>
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C140" s="6"/>
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C141" s="6"/>
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142" s="6"/>
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C143" s="6"/>
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C144" s="6"/>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C145" s="6"/>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C146" s="6"/>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C147" s="6"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C148" s="6"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C150" s="6"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C151" s="6"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C152" s="6"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C153" s="6"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C154" s="6"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C156" s="6"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C157" s="6"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C158" s="6"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C159" s="6"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" s="6"/>
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C161" s="6"/>
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C162" s="6"/>
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C163" s="6"/>
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C164" s="6"/>
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C165" s="6"/>
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C166" s="6"/>
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C167" s="6"/>
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C168" s="6"/>
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C169" s="6"/>
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C170" s="6"/>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C171" s="6"/>
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C173" s="6"/>
       <c r="D173" s="7"/>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C174" s="6"/>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C175" s="6"/>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C176" s="6"/>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C177" s="6"/>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C178" s="6"/>
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C179" s="6"/>
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C180" s="6"/>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C181" s="6"/>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C182" s="6"/>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C183" s="6"/>
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C184" s="6"/>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C185" s="6"/>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C186" s="6"/>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C187" s="6"/>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C188" s="6"/>
       <c r="D188" s="7"/>
     </row>
@@ -11972,25 +11964,25 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -12004,7 +11996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -12018,7 +12010,7 @@
         <v>2750000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>(C5-C4)/7</f>
         <v>4.2857142857142856</v>
@@ -12033,7 +12025,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>(C6-C5)/7+B5</f>
         <v>8.7142857142857153</v>
@@ -12048,7 +12040,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" ref="B7:B10" si="0">(C7-C6)/7+B6</f>
         <v>13.142857142857144</v>
@@ -12063,7 +12055,7 @@
         <v>5800000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>17.142857142857146</v>
@@ -12078,7 +12070,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>21.571428571428577</v>
@@ -12099,7 +12091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>47.714285714285722</v>
@@ -12122,7 +12114,7 @@
         <v>2.2914410879999996E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>(C11-C4+7)/7</f>
         <v>70.285714285714292</v>
@@ -12145,7 +12137,7 @@
         <v>-5.1743121555555611E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>(C12-C4+7)/7</f>
         <v>122.42857142857143</v>
@@ -12168,7 +12160,7 @@
         <v>-0.19130921649999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>(C13-C4+7)/7</f>
         <v>126.85714285714286</v>
@@ -12191,7 +12183,7 @@
         <v>-0.25919076641080624</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" cm="1">
         <f t="array" ref="C36:D36">LINEST(E4:E9,D4:D9)</f>
         <v>9.9142047621025462</v>

</xml_diff>

<commit_message>
Add console print of indiv subreddit estimates; update estimates
</commit_message>
<xml_diff>
--- a/PS VR2 Sales Estimate.xlsx
+++ b/PS VR2 Sales Estimate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aledb\Dropbox (Personal)\Alex\Programming in Python\estimate-PSVR2-sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572B287-81BB-4A63-82F1-91E766E2D640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826D085-C254-460E-8CBF-A03A9980B0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="435" windowWidth="21795" windowHeight="14280" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
+    <workbookView xWindow="990" yWindow="1050" windowWidth="21705" windowHeight="14190" xr2:uid="{64125413-A5F6-4236-BA19-5C5D6C780758}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated PS VR2 Sales" sheetId="5" r:id="rId1"/>
@@ -244,22 +244,18 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -329,10 +325,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$32</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="31"/>
+                  <c:ptCount val="32"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -426,15 +422,18 @@
                   <c:pt idx="30">
                     <c:v>124616.9635824112</c:v>
                   </c:pt>
+                  <c:pt idx="31">
+                    <c:v>125741.26336449782</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$32</c:f>
+                <c:f>'Estimated PS VR2 Sales'!$F$2:$F$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="31"/>
+                  <c:ptCount val="32"/>
                   <c:pt idx="0">
                     <c:v>1511.7424598056805</c:v>
                   </c:pt>
@@ -528,6 +527,9 @@
                   <c:pt idx="30">
                     <c:v>124616.9635824112</c:v>
                   </c:pt>
+                  <c:pt idx="31">
+                    <c:v>125741.26336449782</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
@@ -547,10 +549,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$32</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>44979.791666666664</c:v>
                 </c:pt>
@@ -643,16 +645,19 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>45225</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>45231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$32</c:f>
+              <c:f>'Estimated PS VR2 Sales'!$D$2:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>437221.74996356922</c:v>
                 </c:pt>
@@ -745,6 +750,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>860310.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>865482.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -771,7 +779,7 @@
         <c:axId val="1022667008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45228"/>
+          <c:max val="45238"/>
           <c:min val="44978"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -9691,10 +9699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0C3A37-78ED-4113-9465-0FC068733B9F}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9702,7 +9710,7 @@
     <col min="1" max="1" width="13.28515625" style="12" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="12" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="17" customWidth="1"/>
     <col min="5" max="6" width="12" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
@@ -9735,7 +9743,7 @@
       <c r="C2" s="15">
         <v>436152.78661883302</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <f t="shared" ref="D2:D16" si="0">AVERAGE(B2:C2)</f>
         <v>437221.74996356922</v>
       </c>
@@ -9758,7 +9766,7 @@
       <c r="C3" s="15">
         <v>504280.48190166097</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <f t="shared" si="0"/>
         <v>502628.310008378</v>
       </c>
@@ -9781,7 +9789,7 @@
       <c r="C4" s="15">
         <v>533696.10593416519</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f t="shared" si="0"/>
         <v>533344.70188799629</v>
       </c>
@@ -9804,7 +9812,7 @@
       <c r="C5" s="15">
         <v>549930.20032946218</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>552711.02142206416</v>
       </c>
@@ -9827,7 +9835,7 @@
       <c r="C6" s="15">
         <v>570604.38891834486</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>571084.21920117619</v>
       </c>
@@ -9850,7 +9858,7 @@
       <c r="C7" s="15">
         <v>582537.14206360595</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
         <v>583610.55039985222</v>
       </c>
@@ -9873,7 +9881,7 @@
       <c r="C8" s="15">
         <v>592527.35399917339</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <f t="shared" si="0"/>
         <v>594281.1942206258</v>
       </c>
@@ -9896,7 +9904,7 @@
       <c r="C9" s="15">
         <v>595996.17758791195</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>600857.62877970957</v>
       </c>
@@ -9919,7 +9927,7 @@
       <c r="C10" s="15">
         <v>613062.78964450595</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <f t="shared" si="0"/>
         <v>614315.67281048885</v>
       </c>
@@ -9942,7 +9950,7 @@
       <c r="C11" s="15">
         <v>621526.71920102881</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <f t="shared" si="0"/>
         <v>622651.58592415205</v>
       </c>
@@ -9965,7 +9973,7 @@
       <c r="C12" s="15">
         <v>632349.44879789359</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <f t="shared" si="0"/>
         <v>631727.87202675734</v>
       </c>
@@ -9988,7 +9996,7 @@
       <c r="C13" s="15">
         <v>643310.93133830791</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <f t="shared" si="0"/>
         <v>640669.92786201672</v>
       </c>
@@ -10011,7 +10019,7 @@
       <c r="C14" s="15">
         <v>661626.3198868481</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <f t="shared" si="0"/>
         <v>653638.8857842026</v>
       </c>
@@ -10034,7 +10042,7 @@
       <c r="C15" s="15">
         <v>674114.08480630745</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <f t="shared" si="0"/>
         <v>663821.28610379866</v>
       </c>
@@ -10057,7 +10065,7 @@
       <c r="C16" s="15">
         <v>688960.64976610907</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <f t="shared" si="0"/>
         <v>675246.71354954084</v>
       </c>
@@ -10076,7 +10084,7 @@
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>686000</v>
       </c>
       <c r="E17" s="15">
@@ -10093,7 +10101,7 @@
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>706000</v>
       </c>
       <c r="E18" s="15">
@@ -10110,7 +10118,7 @@
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>716000</v>
       </c>
       <c r="E19" s="15">
@@ -10131,7 +10139,7 @@
       <c r="C20" s="15">
         <v>760695</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>726000</v>
       </c>
       <c r="E20" s="15">
@@ -10152,16 +10160,16 @@
       <c r="C21" s="15">
         <v>787058</v>
       </c>
-      <c r="D21" s="17">
-        <f t="shared" ref="D21:D32" si="3">AVERAGE(B21:C21)</f>
+      <c r="D21" s="16">
+        <f t="shared" ref="D21:D33" si="3">AVERAGE(B21:C21)</f>
         <v>744719.5</v>
       </c>
       <c r="E21" s="15">
-        <f t="shared" ref="E21:E32" si="4">STDEV(B21:C21)*2</f>
+        <f t="shared" ref="E21:E33" si="4">STDEV(B21:C21)*2</f>
         <v>119751.36182106657</v>
       </c>
       <c r="F21" s="15">
-        <f t="shared" ref="F21:F32" si="5">STDEV(B21:C21)</f>
+        <f t="shared" ref="F21:F33" si="5">STDEV(B21:C21)</f>
         <v>59875.680910533287</v>
       </c>
       <c r="H21" s="4"/>
@@ -10176,7 +10184,7 @@
       <c r="C22" s="15">
         <v>800101</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <f t="shared" si="3"/>
         <v>754199.5</v>
       </c>
@@ -10199,7 +10207,7 @@
       <c r="C23" s="15">
         <v>817029</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <f t="shared" si="3"/>
         <v>765921.5</v>
       </c>
@@ -10222,7 +10230,7 @@
       <c r="C24" s="15">
         <v>829101</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <f t="shared" si="3"/>
         <v>775030.5</v>
       </c>
@@ -10245,7 +10253,7 @@
       <c r="C25" s="15">
         <v>838536</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <f t="shared" si="3"/>
         <v>782216.5</v>
       </c>
@@ -10269,7 +10277,7 @@
       <c r="C26" s="15">
         <v>875583</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <f t="shared" si="3"/>
         <v>808852.5</v>
       </c>
@@ -10292,7 +10300,7 @@
       <c r="C27" s="15">
         <v>882659</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="16">
         <f t="shared" si="3"/>
         <v>813892.5</v>
       </c>
@@ -10316,7 +10324,7 @@
       <c r="C28" s="15">
         <v>892372</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <f t="shared" si="3"/>
         <v>820206</v>
       </c>
@@ -10339,7 +10347,7 @@
       <c r="C29" s="15">
         <v>900697</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="16">
         <f t="shared" si="3"/>
         <v>825253</v>
       </c>
@@ -10362,7 +10370,7 @@
       <c r="C30" s="15">
         <v>918735</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="16">
         <f t="shared" si="3"/>
         <v>838458.5</v>
       </c>
@@ -10379,13 +10387,13 @@
       <c r="A31" s="11">
         <v>45217</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="15">
         <v>768197</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="15">
         <v>939132</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="16">
         <f t="shared" si="3"/>
         <v>853664.5</v>
       </c>
@@ -10409,18 +10417,265 @@
       <c r="C32" s="19">
         <v>948428</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="18">
         <f t="shared" si="3"/>
         <v>860310.5</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="19">
         <f t="shared" si="4"/>
         <v>249233.92716482241</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="19">
         <f t="shared" si="5"/>
         <v>124616.9635824112</v>
       </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>45231</v>
+      </c>
+      <c r="B33" s="19">
+        <v>776570</v>
+      </c>
+      <c r="C33" s="19">
+        <v>954395</v>
+      </c>
+      <c r="D33" s="18">
+        <f t="shared" si="3"/>
+        <v>865482.5</v>
+      </c>
+      <c r="E33" s="19">
+        <f t="shared" si="4"/>
+        <v>251482.52672899564</v>
+      </c>
+      <c r="F33" s="19">
+        <f t="shared" si="5"/>
+        <v>125741.26336449782</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>